<commit_message>
added table with conditions for soil in ferre
</commit_message>
<xml_diff>
--- a/ferreSoilConditions.xlsx
+++ b/ferreSoilConditions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="72">
   <si>
     <t>Sands</t>
   </si>
@@ -110,27 +110,12 @@
     <t>7 to 27 percent clay, 28 to 50 percent silt, and 52 percent or less sand.</t>
   </si>
   <si>
-    <t xml:space="preserve">  Silt loam</t>
-  </si>
-  <si>
-    <t>50 percent or more silt and 12 to 27 percent clay, or 50 to 80 percent silt and less than 12 percent clay.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Silt</t>
-  </si>
-  <si>
     <t>80 percent or more silt and less than 12 percent clay.</t>
   </si>
   <si>
-    <t xml:space="preserve">  Sandy clay loam</t>
-  </si>
-  <si>
     <t>20 to 35 percent clay, less than 28 percent silt, and more than 45 percent sand.</t>
   </si>
   <si>
-    <t xml:space="preserve">  Clay loam</t>
-  </si>
-  <si>
     <t>27 to 40 percent clay and more than 20 to 46 percent sand.</t>
   </si>
   <si>
@@ -146,9 +131,6 @@
     <t>40 percent or more clay, 45 percent or less sand, and less than 40 percent silt.</t>
   </si>
   <si>
-    <t>Sand</t>
-  </si>
-  <si>
     <t>&gt;=40</t>
   </si>
   <si>
@@ -164,35 +146,130 @@
     <t xml:space="preserve">  Silty clay Пылеватая глина</t>
   </si>
   <si>
-    <t xml:space="preserve">  Sandy clay Глина песчаная</t>
-  </si>
-  <si>
     <t>Clay Глина</t>
   </si>
   <si>
     <t xml:space="preserve">  Silty clay loam Пылевато-глинистый суглинок</t>
   </si>
   <si>
-    <t>Mud (Clay)</t>
-  </si>
-  <si>
     <t>7-27</t>
   </si>
   <si>
-    <t>Dust (Silt)</t>
-  </si>
-  <si>
     <t>&lt;=52</t>
   </si>
   <si>
     <t>28-50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Sandy clay 
+Глина песчаная</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Clay loam
+Глинистый суглинок</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Sandy clay loam
+Опесчаненный глинистый суглинок</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Silt
+Тонкий суглинок</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Silt loam
+Пылеватый суглинок</t>
+  </si>
+  <si>
+    <t>Sand   Песок</t>
+  </si>
+  <si>
+    <t>&gt;85</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">50 percent or more silt and 12 to 27 percent clay, or 50 to 80 percent silt and less than 12 percent clay.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>&gt;50 пыли и 12-27 глины, или 50-80 пыли и &lt;12 глины</t>
+    </r>
+  </si>
+  <si>
+    <t>(пыль + 1.5*глины) &lt; 15</t>
+  </si>
+  <si>
+    <t>&gt;=80</t>
+  </si>
+  <si>
+    <t>&lt;12</t>
+  </si>
+  <si>
+    <t>Mud (Clay)
+глина</t>
+  </si>
+  <si>
+    <t>Sand
+Песок</t>
+  </si>
+  <si>
+    <t>Dust (Silt)
+Пыль</t>
+  </si>
+  <si>
+    <t>20-35</t>
+  </si>
+  <si>
+    <t>27-40</t>
+  </si>
+  <si>
+    <t>&lt;28</t>
+  </si>
+  <si>
+    <t>&gt;45</t>
+  </si>
+  <si>
+    <t>20-46</t>
+  </si>
+  <si>
+    <t>&lt;=20</t>
+  </si>
+  <si>
+    <t>&gt;=35</t>
+  </si>
+  <si>
+    <t>&gt;=45</t>
+  </si>
+  <si>
+    <t>70-91</t>
+  </si>
+  <si>
+    <t>(пыль + 1.5*глины) &gt;15 и (пыль + 2*глина)&lt;30</t>
+  </si>
+  <si>
+    <t>глина 7-20,  песок &gt; 52, (пыль + 2*глина)&gt;=30  или   глина &lt; 7, пыль &lt; 50, песок &gt;43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Sandy loam
+Опесчаненный суглинок</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Loamy sand
+Суглинистый песок</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,6 +296,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -240,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -255,6 +346,13 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -535,28 +633,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="108.85546875" customWidth="1"/>
+    <col min="2" max="2" width="98.5703125" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" t="s">
-        <v>51</v>
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -643,7 +744,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
     </row>
@@ -671,7 +772,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
@@ -679,7 +780,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="51" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
@@ -687,101 +788,168 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="8"/>
+    </row>
+    <row r="20" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>50</v>
+        <v>71</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>29</v>
+        <v>50</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
+      </c>
+      <c r="C24" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="C25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" t="s">
+        <v>36</v>
+      </c>
+      <c r="E30" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" t="s">
-        <v>42</v>
-      </c>
-      <c r="E28" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>